<commit_message>
adjusted the resolution on the tab bar icon images
</commit_message>
<xml_diff>
--- a/LineUpCard/MissionDataCardMAY19.xlsx
+++ b/LineUpCard/MissionDataCardMAY19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elmo/Dropbox/00_Elmo/05_Coding/03_Working/T38-Beta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elmo/Dropbox/00_Elmo/05_Coding/03_Working/T38-Beta/LineUpCard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A709F0EE-2E87-3746-8C07-3181AF548925}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2988A00D-B892-0E4F-BA36-44A6F120E4B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50580" yWindow="12000" windowWidth="50580" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="25380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mission Data Card" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
   <si>
     <t>TOLD</t>
   </si>
@@ -194,9 +194,6 @@
     <t>#EVENT#</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>#LN1#</t>
   </si>
   <si>
@@ -207,6 +204,24 @@
   </si>
   <si>
     <t>#LN4#</t>
+  </si>
+  <si>
+    <t>#A1#</t>
+  </si>
+  <si>
+    <t>#A2#</t>
+  </si>
+  <si>
+    <t>#A3#</t>
+  </si>
+  <si>
+    <t>#A4#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  /</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -719,12 +734,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -752,65 +761,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
@@ -825,6 +780,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,7 +869,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>489226</xdr:colOff>
+      <xdr:colOff>301078</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>160925</xdr:rowOff>
     </xdr:to>
@@ -1573,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1582,16 +1597,14 @@
     <col min="1" max="1" width="0.83203125" style="26" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="5" max="6" width="6.5" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="40" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="38" customWidth="1"/>
     <col min="10" max="10" width="5.5" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
     <col min="12" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" customWidth="1"/>
+    <col min="14" max="15" width="6.5" customWidth="1"/>
     <col min="16" max="16" width="8.6640625" customWidth="1"/>
     <col min="17" max="17" width="9.33203125" customWidth="1"/>
     <col min="18" max="18" width="8.5" style="26" customWidth="1"/>
@@ -1615,13 +1628,13 @@
       <c r="F2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="43" t="s">
         <v>51</v>
       </c>
       <c r="J2"/>
@@ -1640,13 +1653,13 @@
       <c r="O2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="44" t="s">
+      <c r="Q2" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="43" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1660,17 +1673,19 @@
       <c r="D3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="28"/>
+      <c r="E3" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F3" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="44" t="s">
         <v>56</v>
       </c>
       <c r="J3"/>
@@ -1683,17 +1698,19 @@
       <c r="M3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="28"/>
+      <c r="N3" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="O3" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="44" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1707,17 +1724,19 @@
       <c r="D4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="F4" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="44" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
@@ -1730,17 +1749,19 @@
       <c r="M4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="29"/>
+      <c r="N4" s="29" t="s">
+        <v>62</v>
+      </c>
       <c r="O4" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="43" t="s">
+      <c r="Q4" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="R4" s="46" t="s">
+      <c r="R4" s="44" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1754,18 +1775,20 @@
       <c r="D5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>63</v>
+      </c>
       <c r="F5" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="70" t="s">
-        <v>57</v>
+      <c r="I5" s="50" t="s">
+        <v>65</v>
       </c>
       <c r="J5"/>
       <c r="K5" s="27" t="s">
@@ -1777,23 +1800,25 @@
       <c r="M5" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="33"/>
+      <c r="N5" s="33" t="s">
+        <v>63</v>
+      </c>
       <c r="O5" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="42" t="s">
+      <c r="Q5" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="70" t="s">
-        <v>57</v>
+      <c r="R5" s="50" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:18" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="47" t="s">
-        <v>48</v>
+      <c r="B6" s="45" t="s">
+        <v>66</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>27</v>
@@ -1801,21 +1826,23 @@
       <c r="D6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="34" t="s">
+        <v>64</v>
+      </c>
       <c r="F6" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="71" t="s">
-        <v>57</v>
+      <c r="I6" s="51" t="s">
+        <v>65</v>
       </c>
       <c r="J6"/>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="45" t="s">
         <v>48</v>
       </c>
       <c r="L6" s="34" t="s">
@@ -1824,18 +1851,20 @@
       <c r="M6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="34"/>
+      <c r="N6" s="34" t="s">
+        <v>64</v>
+      </c>
       <c r="O6" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="Q6" s="69" t="s">
+      <c r="Q6" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="71" t="s">
-        <v>57</v>
+      <c r="R6" s="51" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1844,12 +1873,12 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="51"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="4"/>
       <c r="J7"/>
       <c r="K7" s="22" t="s">
@@ -1857,11 +1886,11 @@
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="6"/>
     </row>
@@ -1925,12 +1954,12 @@
     <row r="11" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
       <c r="J11" s="13"/>
       <c r="K11" s="24" t="s">
         <v>5</v>
@@ -1938,65 +1967,65 @@
       <c r="L11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="62"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="64"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="67"/>
     </row>
     <row r="12" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="54"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="61"/>
       <c r="K12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="58"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="65"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="70"/>
     </row>
     <row r="13" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="54"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="61"/>
       <c r="J13" s="13"/>
       <c r="K13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L13" s="38"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="65"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="70"/>
     </row>
     <row r="14" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="54"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="61"/>
       <c r="J14" s="13"/>
       <c r="K14" s="11" t="s">
         <v>2</v>
@@ -2004,22 +2033,22 @@
       <c r="L14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="M14" s="58"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="65"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="70"/>
     </row>
     <row r="15" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="54"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="61"/>
       <c r="J15" s="13"/>
       <c r="K15" s="11" t="s">
         <v>1</v>
@@ -2027,22 +2056,22 @@
       <c r="L15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="58"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="65"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="70"/>
     </row>
     <row r="16" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="54"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="61"/>
       <c r="J16" s="13"/>
       <c r="K16" s="11" t="s">
         <v>3</v>
@@ -2050,22 +2079,22 @@
       <c r="L16" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M16" s="58"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="65"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="70"/>
     </row>
     <row r="17" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="54"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
       <c r="J17"/>
       <c r="K17" s="14" t="s">
         <v>4</v>
@@ -2073,22 +2102,22 @@
       <c r="L17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="58"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="65"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+      <c r="R17" s="70"/>
     </row>
     <row r="18" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="54"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="61"/>
       <c r="J18" s="13"/>
       <c r="K18" s="11" t="s">
         <v>18</v>
@@ -2096,66 +2125,66 @@
       <c r="L18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="58"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="65"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="70"/>
     </row>
     <row r="19" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="54"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="61"/>
       <c r="J19"/>
-      <c r="K19" s="37" t="s">
+      <c r="K19" s="35" t="s">
         <v>17</v>
       </c>
       <c r="L19" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="58"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="65"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="70"/>
     </row>
     <row r="20" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="54"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="61"/>
       <c r="J20"/>
       <c r="K20" s="10" t="s">
         <v>15</v>
       </c>
       <c r="L20" s="19"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="65"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="70"/>
     </row>
     <row r="21" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="54"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="61"/>
       <c r="J21"/>
       <c r="K21" s="11" t="s">
         <v>13</v>
@@ -2163,22 +2192,22 @@
       <c r="L21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="M21" s="58"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="65"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+      <c r="R21" s="70"/>
     </row>
     <row r="22" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="54"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="61"/>
       <c r="J22"/>
       <c r="K22" s="11" t="s">
         <v>14</v>
@@ -2186,111 +2215,111 @@
       <c r="L22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="58"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="65"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
+      <c r="P22" s="69"/>
+      <c r="Q22" s="69"/>
+      <c r="R22" s="70"/>
     </row>
     <row r="23" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="54"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="61"/>
       <c r="J23"/>
-      <c r="K23" s="60" t="s">
+      <c r="K23" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="61" t="s">
+      <c r="L23" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="66"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="68"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="73"/>
     </row>
     <row r="24" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="54"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="61"/>
       <c r="J24"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="64"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="67"/>
     </row>
     <row r="25" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="54"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="61"/>
       <c r="J25"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="65"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="69"/>
+      <c r="R25" s="70"/>
     </row>
     <row r="26" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="54"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="61"/>
       <c r="J26"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="65"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="69"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="69"/>
+      <c r="R26" s="70"/>
     </row>
     <row r="27" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="54"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="61"/>
       <c r="J27"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="65"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="69"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="69"/>
+      <c r="Q27" s="69"/>
+      <c r="R27" s="70"/>
     </row>
     <row r="28" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="24" t="s">
@@ -2299,21 +2328,21 @@
       <c r="C28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="54"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="61"/>
       <c r="J28"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="65"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="69"/>
+      <c r="R28" s="70"/>
     </row>
     <row r="29" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
@@ -2322,42 +2351,42 @@
       <c r="C29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="54"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="61"/>
       <c r="J29"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="65"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+      <c r="R29" s="70"/>
     </row>
     <row r="30" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="54"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="61"/>
       <c r="J30"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
-      <c r="R30" s="65"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="70"/>
     </row>
     <row r="31" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
@@ -2366,21 +2395,21 @@
       <c r="C31" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="54"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="61"/>
       <c r="J31"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="65"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="70"/>
     </row>
     <row r="32" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="11" t="s">
@@ -2389,21 +2418,21 @@
       <c r="C32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="54"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="61"/>
       <c r="J32"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="59"/>
-      <c r="N32" s="59"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="65"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="70"/>
     </row>
     <row r="33" spans="2:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="11" t="s">
@@ -2412,21 +2441,21 @@
       <c r="C33" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="54"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="61"/>
       <c r="J33"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="59"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="65"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="70"/>
     </row>
     <row r="34" spans="2:18" s="2" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
@@ -2435,21 +2464,21 @@
       <c r="C34" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="49"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="54"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="61"/>
       <c r="J34"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="59"/>
-      <c r="N34" s="59"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
-      <c r="R34" s="65"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="69"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="70"/>
     </row>
     <row r="35" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
@@ -2458,65 +2487,65 @@
       <c r="C35" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="54"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="61"/>
       <c r="J35"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="59"/>
-      <c r="M35" s="59"/>
-      <c r="N35" s="59"/>
-      <c r="O35" s="59"/>
-      <c r="P35" s="59"/>
-      <c r="Q35" s="59"/>
-      <c r="R35" s="65"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="70"/>
     </row>
     <row r="36" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="49"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="54"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="61"/>
       <c r="J36"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="65"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="69"/>
+      <c r="R36" s="70"/>
     </row>
     <row r="37" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="19"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="54"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="61"/>
       <c r="J37"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59"/>
-      <c r="R37" s="65"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="69"/>
+      <c r="Q37" s="69"/>
+      <c r="R37" s="70"/>
     </row>
     <row r="38" spans="2:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
@@ -2525,21 +2554,21 @@
       <c r="C38" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
-      <c r="I38" s="54"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="61"/>
       <c r="J38"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="59"/>
-      <c r="R38" s="65"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
+      <c r="Q38" s="69"/>
+      <c r="R38" s="70"/>
     </row>
     <row r="39" spans="2:18" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
@@ -2548,21 +2577,21 @@
       <c r="C39" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="54"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="61"/>
       <c r="J39"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="59"/>
-      <c r="M39" s="59"/>
-      <c r="N39" s="59"/>
-      <c r="O39" s="59"/>
-      <c r="P39" s="59"/>
-      <c r="Q39" s="59"/>
-      <c r="R39" s="65"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="69"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="70"/>
     </row>
     <row r="40" spans="2:18" s="2" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
@@ -2571,21 +2600,21 @@
       <c r="C40" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="57"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="64"/>
       <c r="J40" s="13"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="67"/>
-      <c r="N40" s="67"/>
-      <c r="O40" s="67"/>
-      <c r="P40" s="67"/>
-      <c r="Q40" s="67"/>
-      <c r="R40" s="68"/>
+      <c r="K40" s="71"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="72"/>
+      <c r="N40" s="72"/>
+      <c r="O40" s="72"/>
+      <c r="P40" s="72"/>
+      <c r="Q40" s="72"/>
+      <c r="R40" s="73"/>
     </row>
     <row r="41" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="12" t="s">
@@ -2594,7 +2623,7 @@
       <c r="D41" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="39"/>
+      <c r="I41" s="37"/>
       <c r="K41" s="12" t="s">
         <v>20</v>
       </c>

</xml_diff>